<commit_message>
- fixed compositions reported from `10.1016/j.intermet.2018.05.013`
</commit_message>
<xml_diff>
--- a/HuiSun_FractureToughnessData_Jan2022_AdamFix.xlsx
+++ b/HuiSun_FractureToughnessData_Jan2022_AdamFix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-guest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8643FA93-6AB9-A44F-BA45-F78ADCEC2730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785A0057-79F8-5D40-A59E-AE340C19104E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="322">
   <si>
     <t>Name:</t>
   </si>
@@ -850,9 +850,6 @@
     <t>9</t>
   </si>
   <si>
-    <t>Al16.7 Cr16.7 Fe16.7 Ni33.2 Cu16.8</t>
-  </si>
-  <si>
     <t>8</t>
   </si>
   <si>
@@ -862,13 +859,7 @@
     <t>7</t>
   </si>
   <si>
-    <t>Cr20 Mn20 Fe20 Co20 Ni22</t>
-  </si>
-  <si>
     <t>6</t>
-  </si>
-  <si>
-    <t>Cr20 Mn20 Fe20 Co20 Ni21</t>
   </si>
   <si>
     <t>5</t>
@@ -1822,32 +1813,18 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1900,18 +1877,32 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2196,8 +2187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2231,43 +2222,43 @@
         <v>0</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>322</v>
-      </c>
-      <c r="D2" s="51" t="s">
+        <v>319</v>
+      </c>
+      <c r="D2" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="52"/>
-      <c r="F2" s="47" t="s">
-        <v>324</v>
-      </c>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="48"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="45" t="s">
+        <v>321</v>
+      </c>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="46"/>
       <c r="O2" s="26"/>
     </row>
     <row r="3" spans="1:20" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="70" t="s">
-        <v>323</v>
-      </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="49"/>
-      <c r="N3" s="50"/>
+      <c r="B3" s="44" t="s">
+        <v>320</v>
+      </c>
+      <c r="D3" s="51"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="48"/>
       <c r="O3" s="26"/>
     </row>
     <row r="4" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2285,43 +2276,43 @@
       <c r="B5" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="44" t="s">
+      <c r="D5" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="44" t="s">
+      <c r="E5" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="44" t="s">
+      <c r="F5" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="44" t="s">
+      <c r="G5" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="45" t="s">
+      <c r="H5" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="44" t="s">
+      <c r="I5" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="J5" s="44" t="s">
+      <c r="J5" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="44" t="s">
+      <c r="K5" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="L5" s="44" t="s">
+      <c r="L5" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="44" t="s">
+      <c r="M5" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="N5" s="44" t="s">
+      <c r="N5" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="O5" s="38" t="s">
+      <c r="O5" s="63" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2332,19 +2323,19 @@
       <c r="B6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="44"/>
-      <c r="M6" s="44"/>
-      <c r="N6" s="44"/>
-      <c r="O6" s="39"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="62"/>
+      <c r="L6" s="62"/>
+      <c r="M6" s="62"/>
+      <c r="N6" s="62"/>
+      <c r="O6" s="64"/>
     </row>
     <row r="7" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -2389,7 +2380,7 @@
       <c r="N7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O7" s="40"/>
+      <c r="O7" s="65"/>
       <c r="P7" s="32" t="s">
         <v>40</v>
       </c>
@@ -2402,35 +2393,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="58" t="s">
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="59"/>
-      <c r="H8" s="59"/>
-      <c r="I8" s="59"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="60"/>
-      <c r="L8" s="60"/>
-      <c r="M8" s="61" t="s">
+      <c r="G8" s="57"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="58"/>
+      <c r="K8" s="58"/>
+      <c r="L8" s="58"/>
+      <c r="M8" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="62"/>
+      <c r="N8" s="60"/>
       <c r="O8" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="P8" s="41" t="s">
+      <c r="P8" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="Q8" s="42"/>
-      <c r="R8" s="42"/>
-      <c r="S8" s="42"/>
-      <c r="T8" s="43"/>
+      <c r="Q8" s="67"/>
+      <c r="R8" s="67"/>
+      <c r="S8" s="67"/>
+      <c r="T8" s="68"/>
     </row>
     <row r="9" spans="1:20" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -2494,18 +2485,18 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
       <c r="F10" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G10" s="20" t="s">
         <v>19</v>
@@ -2520,19 +2511,19 @@
       <c r="K10" s="33"/>
       <c r="L10" s="20"/>
       <c r="M10" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N10" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="O10" s="20"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C11" s="20" t="s">
         <v>100</v>
@@ -2540,7 +2531,7 @@
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
       <c r="F11" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G11" s="20" t="s">
         <v>19</v>
@@ -2555,19 +2546,19 @@
       <c r="K11" s="33"/>
       <c r="L11" s="20"/>
       <c r="M11" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N11" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="O11" s="20"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C12" s="20" t="s">
         <v>100</v>
@@ -2575,7 +2566,7 @@
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
       <c r="F12" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G12" s="20" t="s">
         <v>19</v>
@@ -2590,19 +2581,19 @@
       <c r="K12" s="33"/>
       <c r="L12" s="20"/>
       <c r="M12" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N12" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="O12" s="21"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C13" s="20" t="s">
         <v>121</v>
@@ -2610,7 +2601,7 @@
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
       <c r="F13" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G13" s="20" t="s">
         <v>19</v>
@@ -2625,19 +2616,19 @@
       <c r="K13" s="33"/>
       <c r="L13" s="20"/>
       <c r="M13" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N13" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="O13" s="20"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C14" s="20" t="s">
         <v>121</v>
@@ -2645,7 +2636,7 @@
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
       <c r="F14" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>19</v>
@@ -2660,19 +2651,19 @@
       <c r="K14" s="33"/>
       <c r="L14" s="20"/>
       <c r="M14" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N14" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="O14" s="20"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="B15" s="20" t="s">
         <v>239</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>238</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>121</v>
@@ -2680,7 +2671,7 @@
       <c r="D15" s="20"/>
       <c r="E15" s="20"/>
       <c r="F15" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G15" s="20" t="s">
         <v>19</v>
@@ -2695,19 +2686,19 @@
       <c r="K15" s="33"/>
       <c r="L15" s="20"/>
       <c r="M15" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N15" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="O15" s="20"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C16" s="20" t="s">
         <v>227</v>
@@ -2715,7 +2706,7 @@
       <c r="D16" s="20"/>
       <c r="E16" s="20"/>
       <c r="F16" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G16" s="20" t="s">
         <v>19</v>
@@ -2730,31 +2721,31 @@
       <c r="K16" s="33"/>
       <c r="L16" s="20"/>
       <c r="M16" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N16" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="O16" s="20"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="B17" s="20" t="s">
         <v>235</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>234</v>
       </c>
       <c r="C17" s="20" t="s">
         <v>227</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G17" s="20" t="s">
         <v>19</v>
       </c>
       <c r="H17" s="34"/>
-      <c r="I17" s="67">
+      <c r="I17" s="41">
         <v>473</v>
       </c>
       <c r="J17">
@@ -2763,10 +2754,10 @@
       <c r="K17" s="33"/>
       <c r="L17" s="20"/>
       <c r="M17" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N17" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
@@ -2780,7 +2771,7 @@
         <v>227</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G18" s="20" t="s">
         <v>19</v>
@@ -2795,10 +2786,10 @@
       <c r="K18" s="33"/>
       <c r="L18" s="20"/>
       <c r="M18" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N18" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
@@ -2812,7 +2803,7 @@
         <v>100</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G19" s="20" t="s">
         <v>19</v>
@@ -2827,10 +2818,10 @@
       <c r="K19" s="33"/>
       <c r="L19" s="20"/>
       <c r="M19" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N19" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
@@ -2844,7 +2835,7 @@
         <v>227</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G20" s="20" t="s">
         <v>19</v>
@@ -2859,10 +2850,10 @@
       <c r="K20" s="33"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N20" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
@@ -2876,7 +2867,7 @@
         <v>121</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G21" s="20" t="s">
         <v>19</v>
@@ -2891,10 +2882,10 @@
       <c r="K21" s="33"/>
       <c r="L21" s="20"/>
       <c r="M21" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N21" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
@@ -2908,7 +2899,7 @@
         <v>121</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G22" s="20" t="s">
         <v>19</v>
@@ -2923,10 +2914,10 @@
       <c r="K22" s="33"/>
       <c r="L22" s="20"/>
       <c r="M22" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N22" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
@@ -2940,7 +2931,7 @@
         <v>121</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G23" s="20" t="s">
         <v>19</v>
@@ -2955,10 +2946,10 @@
       <c r="K23" s="33"/>
       <c r="L23" s="20"/>
       <c r="M23" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N23" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
@@ -2972,7 +2963,7 @@
         <v>121</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G24" s="20" t="s">
         <v>19</v>
@@ -2987,10 +2978,10 @@
       <c r="K24" s="33"/>
       <c r="L24" s="20"/>
       <c r="M24" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N24" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
@@ -3004,10 +2995,10 @@
         <v>100</v>
       </c>
       <c r="E25" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G25" s="20" t="s">
         <v>19</v>
@@ -3022,10 +3013,10 @@
       <c r="K25" s="33"/>
       <c r="L25" s="20"/>
       <c r="M25" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N25" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
@@ -3039,10 +3030,10 @@
         <v>217</v>
       </c>
       <c r="E26" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G26" s="20" t="s">
         <v>19</v>
@@ -3057,10 +3048,10 @@
       <c r="K26" s="33"/>
       <c r="L26" s="20"/>
       <c r="M26" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
@@ -3074,7 +3065,7 @@
         <v>100</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G27" s="20" t="s">
         <v>19</v>
@@ -3089,10 +3080,10 @@
       <c r="K27" s="33"/>
       <c r="L27" s="20"/>
       <c r="M27" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N27" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
@@ -3106,7 +3097,7 @@
         <v>100</v>
       </c>
       <c r="F28" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G28" s="20" t="s">
         <v>19</v>
@@ -3121,10 +3112,10 @@
       <c r="K28" s="33"/>
       <c r="L28" s="20"/>
       <c r="M28" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N28" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
@@ -3138,7 +3129,7 @@
         <v>100</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G29" s="20" t="s">
         <v>19</v>
@@ -3153,10 +3144,10 @@
       <c r="K29" s="33"/>
       <c r="L29" s="20"/>
       <c r="M29" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N29" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
@@ -3170,7 +3161,7 @@
         <v>100</v>
       </c>
       <c r="F30" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G30" s="20" t="s">
         <v>19</v>
@@ -3185,10 +3176,10 @@
       <c r="K30" s="33"/>
       <c r="L30" s="20"/>
       <c r="M30" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N30" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -3202,7 +3193,7 @@
         <v>121</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G31" s="20" t="s">
         <v>19</v>
@@ -3217,10 +3208,10 @@
       <c r="K31" s="33"/>
       <c r="L31" s="20"/>
       <c r="M31" s="20" t="s">
-        <v>279</v>
-      </c>
-      <c r="N31" s="69" t="s">
-        <v>319</v>
+        <v>276</v>
+      </c>
+      <c r="N31" s="43" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -3234,7 +3225,7 @@
         <v>121</v>
       </c>
       <c r="F32" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G32" s="20" t="s">
         <v>19</v>
@@ -3249,10 +3240,10 @@
       <c r="K32" s="33"/>
       <c r="L32" s="20"/>
       <c r="M32" s="20" t="s">
-        <v>279</v>
-      </c>
-      <c r="N32" s="69" t="s">
-        <v>319</v>
+        <v>276</v>
+      </c>
+      <c r="N32" s="43" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
@@ -3266,7 +3257,7 @@
         <v>100</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G33" s="20" t="s">
         <v>19</v>
@@ -3281,10 +3272,10 @@
       <c r="K33" s="33"/>
       <c r="L33" s="20"/>
       <c r="M33" s="20" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="N33" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -3294,11 +3285,11 @@
       <c r="B34" s="20" t="s">
         <v>202</v>
       </c>
-      <c r="C34" s="66" t="s">
+      <c r="C34" s="40" t="s">
         <v>118</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G34" s="20" t="s">
         <v>19</v>
@@ -3313,10 +3304,10 @@
       <c r="K34" s="33"/>
       <c r="L34" s="20"/>
       <c r="M34" s="20" t="s">
-        <v>276</v>
-      </c>
-      <c r="N34" s="68" t="s">
-        <v>317</v>
+        <v>273</v>
+      </c>
+      <c r="N34" s="42" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -3326,11 +3317,11 @@
       <c r="B35" s="20" t="s">
         <v>200</v>
       </c>
-      <c r="C35" s="66" t="s">
+      <c r="C35" s="40" t="s">
         <v>118</v>
       </c>
       <c r="F35" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G35" s="20" t="s">
         <v>19</v>
@@ -3345,10 +3336,10 @@
       <c r="K35" s="33"/>
       <c r="L35" s="20"/>
       <c r="M35" s="20" t="s">
-        <v>276</v>
-      </c>
-      <c r="N35" s="68" t="s">
-        <v>317</v>
+        <v>273</v>
+      </c>
+      <c r="N35" s="42" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -3358,11 +3349,11 @@
       <c r="B36" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="C36" s="66" t="s">
+      <c r="C36" s="40" t="s">
         <v>118</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G36" s="20" t="s">
         <v>19</v>
@@ -3377,10 +3368,10 @@
       <c r="K36" s="33"/>
       <c r="L36" s="20"/>
       <c r="M36" s="20" t="s">
-        <v>276</v>
-      </c>
-      <c r="N36" s="68" t="s">
-        <v>317</v>
+        <v>273</v>
+      </c>
+      <c r="N36" s="42" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -3390,14 +3381,14 @@
       <c r="B37" s="20" t="s">
         <v>196</v>
       </c>
-      <c r="C37" s="66" t="s">
+      <c r="C37" s="40" t="s">
         <v>195</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G37" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="H37" s="34"/>
       <c r="J37">
@@ -3406,10 +3397,10 @@
       <c r="K37" s="33"/>
       <c r="L37" s="20"/>
       <c r="M37" s="20" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="N37" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -3419,11 +3410,11 @@
       <c r="B38" s="20" t="s">
         <v>192</v>
       </c>
-      <c r="C38" s="66" t="s">
+      <c r="C38" s="40" t="s">
         <v>100</v>
       </c>
       <c r="F38" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G38" s="20" t="s">
         <v>19</v>
@@ -3438,10 +3429,10 @@
       <c r="K38" s="33"/>
       <c r="L38" s="20"/>
       <c r="M38" s="20" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="N38" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -3451,11 +3442,11 @@
       <c r="B39" s="20" t="s">
         <v>192</v>
       </c>
-      <c r="C39" s="66" t="s">
+      <c r="C39" s="40" t="s">
         <v>100</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G39" s="20" t="s">
         <v>19</v>
@@ -3470,10 +3461,10 @@
       <c r="K39" s="33"/>
       <c r="L39" s="20"/>
       <c r="M39" s="20" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="N39" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
@@ -3487,13 +3478,13 @@
         <v>100</v>
       </c>
       <c r="F40" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G40" s="20" t="s">
         <v>19</v>
       </c>
       <c r="H40" s="34"/>
-      <c r="I40" s="67">
+      <c r="I40" s="41">
         <v>296</v>
       </c>
       <c r="J40">
@@ -3502,10 +3493,10 @@
       <c r="K40" s="33"/>
       <c r="L40" s="20"/>
       <c r="M40" s="20" t="s">
-        <v>292</v>
-      </c>
-      <c r="N40" s="68" t="s">
-        <v>314</v>
+        <v>289</v>
+      </c>
+      <c r="N40" s="42" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -3515,23 +3506,23 @@
       <c r="B41" s="20" t="s">
         <v>190</v>
       </c>
-      <c r="C41" s="66" t="s">
+      <c r="C41" s="40" t="s">
         <v>126</v>
       </c>
       <c r="D41" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E41" t="s">
+        <v>266</v>
+      </c>
+      <c r="F41" s="20" t="s">
         <v>269</v>
-      </c>
-      <c r="F41" s="20" t="s">
-        <v>272</v>
       </c>
       <c r="G41" s="20" t="s">
         <v>19</v>
       </c>
       <c r="H41" s="34"/>
-      <c r="I41" s="67">
+      <c r="I41" s="41">
         <v>296</v>
       </c>
       <c r="J41">
@@ -3540,10 +3531,10 @@
       <c r="K41" s="33"/>
       <c r="L41" s="20"/>
       <c r="M41" s="20" t="s">
-        <v>278</v>
-      </c>
-      <c r="N41" s="68" t="s">
-        <v>314</v>
+        <v>275</v>
+      </c>
+      <c r="N41" s="42" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -3553,23 +3544,23 @@
       <c r="B42" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="C42" s="66" t="s">
+      <c r="C42" s="40" t="s">
         <v>126</v>
       </c>
       <c r="D42" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E42" t="s">
+        <v>266</v>
+      </c>
+      <c r="F42" s="20" t="s">
         <v>269</v>
-      </c>
-      <c r="F42" s="20" t="s">
-        <v>272</v>
       </c>
       <c r="G42" s="20" t="s">
         <v>19</v>
       </c>
       <c r="H42" s="34"/>
-      <c r="I42" s="67">
+      <c r="I42" s="41">
         <v>296</v>
       </c>
       <c r="J42">
@@ -3578,10 +3569,10 @@
       <c r="K42" s="33"/>
       <c r="L42" s="20"/>
       <c r="M42" s="20" t="s">
-        <v>278</v>
-      </c>
-      <c r="N42" s="68" t="s">
-        <v>314</v>
+        <v>275</v>
+      </c>
+      <c r="N42" s="42" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -3591,23 +3582,23 @@
       <c r="B43" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="C43" s="66" t="s">
+      <c r="C43" s="40" t="s">
         <v>126</v>
       </c>
       <c r="D43" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E43" t="s">
+        <v>266</v>
+      </c>
+      <c r="F43" s="20" t="s">
         <v>269</v>
-      </c>
-      <c r="F43" s="20" t="s">
-        <v>272</v>
       </c>
       <c r="G43" s="20" t="s">
         <v>19</v>
       </c>
       <c r="H43" s="34"/>
-      <c r="I43" s="67">
+      <c r="I43" s="41">
         <v>296</v>
       </c>
       <c r="J43">
@@ -3616,10 +3607,10 @@
       <c r="K43" s="33"/>
       <c r="L43" s="20"/>
       <c r="M43" s="20" t="s">
-        <v>278</v>
-      </c>
-      <c r="N43" s="68" t="s">
-        <v>314</v>
+        <v>275</v>
+      </c>
+      <c r="N43" s="42" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -3629,23 +3620,23 @@
       <c r="B44" s="20" t="s">
         <v>184</v>
       </c>
-      <c r="C44" s="66" t="s">
+      <c r="C44" s="40" t="s">
         <v>126</v>
       </c>
       <c r="D44" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E44" t="s">
+        <v>266</v>
+      </c>
+      <c r="F44" s="20" t="s">
         <v>269</v>
-      </c>
-      <c r="F44" s="20" t="s">
-        <v>272</v>
       </c>
       <c r="G44" s="20" t="s">
         <v>19</v>
       </c>
       <c r="H44" s="34"/>
-      <c r="I44" s="67">
+      <c r="I44" s="41">
         <v>296</v>
       </c>
       <c r="J44">
@@ -3654,10 +3645,10 @@
       <c r="K44" s="33"/>
       <c r="L44" s="20"/>
       <c r="M44" s="20" t="s">
-        <v>278</v>
-      </c>
-      <c r="N44" s="68" t="s">
-        <v>314</v>
+        <v>275</v>
+      </c>
+      <c r="N44" s="42" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -3667,23 +3658,23 @@
       <c r="B45" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="C45" s="66" t="s">
+      <c r="C45" s="40" t="s">
         <v>126</v>
       </c>
       <c r="D45" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E45" t="s">
+        <v>266</v>
+      </c>
+      <c r="F45" s="20" t="s">
         <v>269</v>
-      </c>
-      <c r="F45" s="20" t="s">
-        <v>272</v>
       </c>
       <c r="G45" s="20" t="s">
         <v>19</v>
       </c>
       <c r="H45" s="34"/>
-      <c r="I45" s="67">
+      <c r="I45" s="41">
         <v>223</v>
       </c>
       <c r="J45">
@@ -3692,10 +3683,10 @@
       <c r="K45" s="33"/>
       <c r="L45" s="20"/>
       <c r="M45" s="20" t="s">
-        <v>278</v>
-      </c>
-      <c r="N45" s="68" t="s">
-        <v>314</v>
+        <v>275</v>
+      </c>
+      <c r="N45" s="42" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -3705,23 +3696,23 @@
       <c r="B46" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="C46" s="66" t="s">
+      <c r="C46" s="40" t="s">
         <v>126</v>
       </c>
       <c r="D46" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E46" t="s">
+        <v>266</v>
+      </c>
+      <c r="F46" s="20" t="s">
         <v>269</v>
-      </c>
-      <c r="F46" s="20" t="s">
-        <v>272</v>
       </c>
       <c r="G46" s="20" t="s">
         <v>19</v>
       </c>
       <c r="H46" s="34"/>
-      <c r="I46" s="67">
+      <c r="I46" s="41">
         <v>223</v>
       </c>
       <c r="J46">
@@ -3730,10 +3721,10 @@
       <c r="K46" s="33"/>
       <c r="L46" s="20"/>
       <c r="M46" s="20" t="s">
-        <v>278</v>
-      </c>
-      <c r="N46" s="68" t="s">
-        <v>314</v>
+        <v>275</v>
+      </c>
+      <c r="N46" s="42" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -3743,23 +3734,23 @@
       <c r="B47" s="20" t="s">
         <v>184</v>
       </c>
-      <c r="C47" s="66" t="s">
+      <c r="C47" s="40" t="s">
         <v>126</v>
       </c>
       <c r="D47" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E47" t="s">
+        <v>266</v>
+      </c>
+      <c r="F47" s="20" t="s">
         <v>269</v>
-      </c>
-      <c r="F47" s="20" t="s">
-        <v>272</v>
       </c>
       <c r="G47" s="20" t="s">
         <v>19</v>
       </c>
       <c r="H47" s="34"/>
-      <c r="I47" s="67">
+      <c r="I47" s="41">
         <v>223</v>
       </c>
       <c r="J47">
@@ -3768,10 +3759,10 @@
       <c r="K47" s="33"/>
       <c r="L47" s="20"/>
       <c r="M47" s="20" t="s">
-        <v>278</v>
-      </c>
-      <c r="N47" s="68" t="s">
-        <v>314</v>
+        <v>275</v>
+      </c>
+      <c r="N47" s="42" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -3781,23 +3772,23 @@
       <c r="B48" s="20" t="s">
         <v>190</v>
       </c>
-      <c r="C48" s="66" t="s">
+      <c r="C48" s="40" t="s">
         <v>126</v>
       </c>
       <c r="D48" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E48" t="s">
+        <v>266</v>
+      </c>
+      <c r="F48" s="20" t="s">
         <v>269</v>
-      </c>
-      <c r="F48" s="20" t="s">
-        <v>272</v>
       </c>
       <c r="G48" s="20" t="s">
         <v>19</v>
       </c>
       <c r="H48" s="34"/>
-      <c r="I48" s="67">
+      <c r="I48" s="41">
         <v>173</v>
       </c>
       <c r="J48">
@@ -3806,10 +3797,10 @@
       <c r="K48" s="33"/>
       <c r="L48" s="20"/>
       <c r="M48" s="20" t="s">
-        <v>278</v>
-      </c>
-      <c r="N48" s="68" t="s">
-        <v>314</v>
+        <v>275</v>
+      </c>
+      <c r="N48" s="42" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -3819,23 +3810,23 @@
       <c r="B49" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="C49" s="66" t="s">
+      <c r="C49" s="40" t="s">
         <v>126</v>
       </c>
       <c r="D49" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E49" t="s">
+        <v>266</v>
+      </c>
+      <c r="F49" s="20" t="s">
         <v>269</v>
-      </c>
-      <c r="F49" s="20" t="s">
-        <v>272</v>
       </c>
       <c r="G49" s="20" t="s">
         <v>19</v>
       </c>
       <c r="H49" s="34"/>
-      <c r="I49" s="67">
+      <c r="I49" s="41">
         <v>173</v>
       </c>
       <c r="J49">
@@ -3844,10 +3835,10 @@
       <c r="K49" s="33"/>
       <c r="L49" s="20"/>
       <c r="M49" s="20" t="s">
-        <v>278</v>
-      </c>
-      <c r="N49" s="68" t="s">
-        <v>314</v>
+        <v>275</v>
+      </c>
+      <c r="N49" s="42" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -3857,23 +3848,23 @@
       <c r="B50" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="C50" s="66" t="s">
+      <c r="C50" s="40" t="s">
         <v>126</v>
       </c>
       <c r="D50" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E50" t="s">
+        <v>266</v>
+      </c>
+      <c r="F50" s="20" t="s">
         <v>269</v>
-      </c>
-      <c r="F50" s="20" t="s">
-        <v>272</v>
       </c>
       <c r="G50" s="20" t="s">
         <v>19</v>
       </c>
       <c r="H50" s="34"/>
-      <c r="I50" s="67">
+      <c r="I50" s="41">
         <v>173</v>
       </c>
       <c r="J50">
@@ -3882,10 +3873,10 @@
       <c r="K50" s="33"/>
       <c r="L50" s="20"/>
       <c r="M50" s="20" t="s">
-        <v>278</v>
-      </c>
-      <c r="N50" s="68" t="s">
-        <v>314</v>
+        <v>275</v>
+      </c>
+      <c r="N50" s="42" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -3895,23 +3886,23 @@
       <c r="B51" s="20" t="s">
         <v>184</v>
       </c>
-      <c r="C51" s="66" t="s">
+      <c r="C51" s="40" t="s">
         <v>126</v>
       </c>
       <c r="D51" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E51" t="s">
+        <v>266</v>
+      </c>
+      <c r="F51" s="20" t="s">
         <v>269</v>
-      </c>
-      <c r="F51" s="20" t="s">
-        <v>272</v>
       </c>
       <c r="G51" s="20" t="s">
         <v>19</v>
       </c>
       <c r="H51" s="34"/>
-      <c r="I51" s="67">
+      <c r="I51" s="41">
         <v>173</v>
       </c>
       <c r="J51">
@@ -3920,10 +3911,10 @@
       <c r="K51" s="33"/>
       <c r="L51" s="20"/>
       <c r="M51" s="20" t="s">
-        <v>278</v>
-      </c>
-      <c r="N51" s="68" t="s">
-        <v>314</v>
+        <v>275</v>
+      </c>
+      <c r="N51" s="42" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -3933,35 +3924,35 @@
       <c r="B52" s="20" t="s">
         <v>190</v>
       </c>
-      <c r="C52" s="66" t="s">
+      <c r="C52" s="40" t="s">
         <v>126</v>
       </c>
       <c r="D52" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E52" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F52" s="20" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="G52" s="20" t="s">
         <v>19</v>
       </c>
       <c r="H52" s="34"/>
-      <c r="I52" s="67">
+      <c r="I52" s="41">
         <v>296</v>
       </c>
-      <c r="J52" s="67">
+      <c r="J52" s="41">
         <v>621000000</v>
       </c>
       <c r="K52" s="33"/>
       <c r="L52" s="20"/>
       <c r="M52" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="N52" s="68" t="s">
-        <v>314</v>
+        <v>280</v>
+      </c>
+      <c r="N52" s="42" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="53" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -3971,35 +3962,35 @@
       <c r="B53" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="C53" s="66" t="s">
+      <c r="C53" s="40" t="s">
         <v>126</v>
       </c>
       <c r="D53" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E53" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F53" s="20" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="G53" s="20" t="s">
         <v>19</v>
       </c>
       <c r="H53" s="34"/>
-      <c r="I53" s="67">
+      <c r="I53" s="41">
         <v>296</v>
       </c>
-      <c r="J53" s="67">
+      <c r="J53" s="41">
         <v>616000000</v>
       </c>
       <c r="K53" s="33"/>
       <c r="L53" s="20"/>
       <c r="M53" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="N53" s="68" t="s">
-        <v>314</v>
+        <v>280</v>
+      </c>
+      <c r="N53" s="42" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -4009,35 +4000,35 @@
       <c r="B54" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="C54" s="66" t="s">
+      <c r="C54" s="40" t="s">
         <v>126</v>
       </c>
       <c r="D54" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E54" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F54" s="20" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="G54" s="20" t="s">
         <v>19</v>
       </c>
       <c r="H54" s="34"/>
-      <c r="I54" s="67">
+      <c r="I54" s="41">
         <v>296</v>
       </c>
-      <c r="J54" s="67">
+      <c r="J54" s="41">
         <v>600000000</v>
       </c>
       <c r="K54" s="33"/>
       <c r="L54" s="20"/>
       <c r="M54" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="N54" s="68" t="s">
-        <v>314</v>
+        <v>280</v>
+      </c>
+      <c r="N54" s="42" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="55" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -4047,35 +4038,35 @@
       <c r="B55" s="20" t="s">
         <v>184</v>
       </c>
-      <c r="C55" s="66" t="s">
+      <c r="C55" s="40" t="s">
         <v>126</v>
       </c>
       <c r="D55" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E55" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F55" s="20" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="G55" s="20" t="s">
         <v>19</v>
       </c>
       <c r="H55" s="34"/>
-      <c r="I55" s="67">
+      <c r="I55" s="41">
         <v>296</v>
       </c>
-      <c r="J55" s="67">
+      <c r="J55" s="41">
         <v>594000000</v>
       </c>
       <c r="K55" s="33"/>
       <c r="L55" s="20"/>
       <c r="M55" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="N55" s="68" t="s">
-        <v>314</v>
+        <v>280</v>
+      </c>
+      <c r="N55" s="42" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="56" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -4085,17 +4076,17 @@
       <c r="B56" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="C56" s="66" t="s">
+      <c r="C56" s="40" t="s">
         <v>157</v>
       </c>
       <c r="D56" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="E56" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F56" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G56" s="20" t="s">
         <v>19</v>
@@ -4107,10 +4098,10 @@
       <c r="K56" s="33"/>
       <c r="L56" s="20"/>
       <c r="M56" s="20" t="s">
-        <v>275</v>
-      </c>
-      <c r="N56" s="68" t="s">
-        <v>313</v>
+        <v>272</v>
+      </c>
+      <c r="N56" s="42" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="57" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -4120,17 +4111,17 @@
       <c r="B57" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="C57" s="66" t="s">
+      <c r="C57" s="40" t="s">
         <v>157</v>
       </c>
       <c r="D57" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="E57" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F57" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G57" s="20" t="s">
         <v>19</v>
@@ -4142,10 +4133,10 @@
       <c r="K57" s="33"/>
       <c r="L57" s="20"/>
       <c r="M57" s="20" t="s">
-        <v>275</v>
-      </c>
-      <c r="N57" s="68" t="s">
-        <v>313</v>
+        <v>272</v>
+      </c>
+      <c r="N57" s="42" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -4155,17 +4146,17 @@
       <c r="B58" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="C58" s="66" t="s">
+      <c r="C58" s="40" t="s">
         <v>157</v>
       </c>
       <c r="D58" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="E58" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F58" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G58" s="20" t="s">
         <v>19</v>
@@ -4177,10 +4168,10 @@
       <c r="K58" s="33"/>
       <c r="L58" s="20"/>
       <c r="M58" s="20" t="s">
-        <v>275</v>
-      </c>
-      <c r="N58" s="68" t="s">
-        <v>313</v>
+        <v>272</v>
+      </c>
+      <c r="N58" s="42" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="59" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -4190,17 +4181,17 @@
       <c r="B59" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="C59" s="66" t="s">
+      <c r="C59" s="40" t="s">
         <v>157</v>
       </c>
       <c r="D59" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="E59" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F59" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G59" s="20" t="s">
         <v>19</v>
@@ -4212,10 +4203,10 @@
       <c r="K59" s="33"/>
       <c r="L59" s="20"/>
       <c r="M59" s="20" t="s">
-        <v>275</v>
-      </c>
-      <c r="N59" s="68" t="s">
-        <v>313</v>
+        <v>272</v>
+      </c>
+      <c r="N59" s="42" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="60" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -4225,17 +4216,17 @@
       <c r="B60" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="C60" s="66" t="s">
+      <c r="C60" s="40" t="s">
         <v>157</v>
       </c>
       <c r="D60" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E60" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F60" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G60" s="20" t="s">
         <v>19</v>
@@ -4247,10 +4238,10 @@
       <c r="K60" s="33"/>
       <c r="L60" s="20"/>
       <c r="M60" s="20" t="s">
-        <v>275</v>
-      </c>
-      <c r="N60" s="68" t="s">
-        <v>313</v>
+        <v>272</v>
+      </c>
+      <c r="N60" s="42" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="61" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -4260,17 +4251,17 @@
       <c r="B61" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="C61" s="66" t="s">
+      <c r="C61" s="40" t="s">
         <v>157</v>
       </c>
       <c r="D61" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E61" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F61" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G61" s="20" t="s">
         <v>19</v>
@@ -4282,10 +4273,10 @@
       <c r="K61" s="33"/>
       <c r="L61" s="20"/>
       <c r="M61" s="20" t="s">
-        <v>275</v>
-      </c>
-      <c r="N61" s="68" t="s">
-        <v>313</v>
+        <v>272</v>
+      </c>
+      <c r="N61" s="42" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="62" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -4295,17 +4286,17 @@
       <c r="B62" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="C62" s="66" t="s">
+      <c r="C62" s="40" t="s">
         <v>157</v>
       </c>
       <c r="D62" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="E62" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F62" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G62" s="20" t="s">
         <v>19</v>
@@ -4317,10 +4308,10 @@
       <c r="K62" s="33"/>
       <c r="L62" s="20"/>
       <c r="M62" s="20" t="s">
-        <v>275</v>
-      </c>
-      <c r="N62" s="68" t="s">
-        <v>313</v>
+        <v>272</v>
+      </c>
+      <c r="N62" s="42" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="63" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -4330,14 +4321,14 @@
       <c r="B63" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="C63" s="66" t="s">
+      <c r="C63" s="40" t="s">
         <v>157</v>
       </c>
       <c r="D63" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F63" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G63" s="20" t="s">
         <v>19</v>
@@ -4349,10 +4340,10 @@
       <c r="K63" s="33"/>
       <c r="L63" s="20"/>
       <c r="M63" s="20" t="s">
-        <v>291</v>
-      </c>
-      <c r="N63" s="68" t="s">
-        <v>313</v>
+        <v>288</v>
+      </c>
+      <c r="N63" s="42" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="64" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -4362,14 +4353,14 @@
       <c r="B64" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="C64" s="66" t="s">
+      <c r="C64" s="40" t="s">
         <v>157</v>
       </c>
       <c r="D64" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F64" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G64" s="20" t="s">
         <v>19</v>
@@ -4381,10 +4372,10 @@
       <c r="K64" s="33"/>
       <c r="L64" s="20"/>
       <c r="M64" s="20" t="s">
-        <v>291</v>
-      </c>
-      <c r="N64" s="68" t="s">
-        <v>313</v>
+        <v>288</v>
+      </c>
+      <c r="N64" s="42" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="65" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -4394,14 +4385,14 @@
       <c r="B65" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="C65" s="66" t="s">
+      <c r="C65" s="40" t="s">
         <v>157</v>
       </c>
       <c r="D65" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F65" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G65" s="20" t="s">
         <v>19</v>
@@ -4413,10 +4404,10 @@
       <c r="K65" s="33"/>
       <c r="L65" s="20"/>
       <c r="M65" s="20" t="s">
-        <v>291</v>
-      </c>
-      <c r="N65" s="68" t="s">
-        <v>313</v>
+        <v>288</v>
+      </c>
+      <c r="N65" s="42" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="66" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -4426,14 +4417,14 @@
       <c r="B66" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="C66" s="66" t="s">
+      <c r="C66" s="40" t="s">
         <v>157</v>
       </c>
       <c r="D66" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F66" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G66" s="20" t="s">
         <v>19</v>
@@ -4445,10 +4436,10 @@
       <c r="K66" s="33"/>
       <c r="L66" s="20"/>
       <c r="M66" s="20" t="s">
-        <v>291</v>
-      </c>
-      <c r="N66" s="68" t="s">
-        <v>313</v>
+        <v>288</v>
+      </c>
+      <c r="N66" s="42" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="67" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -4458,14 +4449,14 @@
       <c r="B67" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="C67" s="66" t="s">
+      <c r="C67" s="40" t="s">
         <v>157</v>
       </c>
       <c r="D67" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F67" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G67" s="20" t="s">
         <v>19</v>
@@ -4477,10 +4468,10 @@
       <c r="K67" s="33"/>
       <c r="L67" s="20"/>
       <c r="M67" s="20" t="s">
-        <v>291</v>
-      </c>
-      <c r="N67" s="68" t="s">
-        <v>313</v>
+        <v>288</v>
+      </c>
+      <c r="N67" s="42" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="68" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -4490,14 +4481,14 @@
       <c r="B68" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="C68" s="66" t="s">
+      <c r="C68" s="40" t="s">
         <v>157</v>
       </c>
       <c r="D68" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F68" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G68" s="20" t="s">
         <v>19</v>
@@ -4509,10 +4500,10 @@
       <c r="K68" s="33"/>
       <c r="L68" s="20"/>
       <c r="M68" s="20" t="s">
-        <v>291</v>
-      </c>
-      <c r="N68" s="68" t="s">
-        <v>313</v>
+        <v>288</v>
+      </c>
+      <c r="N68" s="42" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
@@ -4526,10 +4517,10 @@
         <v>152</v>
       </c>
       <c r="D69" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F69" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G69" s="20" t="s">
         <v>19</v>
@@ -4544,10 +4535,10 @@
       <c r="K69" s="33"/>
       <c r="L69" s="20"/>
       <c r="M69" s="20" t="s">
-        <v>290</v>
-      </c>
-      <c r="N69" s="68" t="s">
-        <v>312</v>
+        <v>287</v>
+      </c>
+      <c r="N69" s="42" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
@@ -4561,10 +4552,10 @@
         <v>152</v>
       </c>
       <c r="D70" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F70" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G70" s="20" t="s">
         <v>19</v>
@@ -4579,10 +4570,10 @@
       <c r="K70" s="33"/>
       <c r="L70" s="20"/>
       <c r="M70" s="20" t="s">
-        <v>290</v>
-      </c>
-      <c r="N70" s="68" t="s">
-        <v>312</v>
+        <v>287</v>
+      </c>
+      <c r="N70" s="42" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
@@ -4593,7 +4584,7 @@
         <v>150</v>
       </c>
       <c r="F71" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G71" s="20" t="s">
         <v>19</v>
@@ -4608,10 +4599,10 @@
       <c r="K71" s="33"/>
       <c r="L71" s="20"/>
       <c r="M71" s="20" t="s">
-        <v>290</v>
-      </c>
-      <c r="N71" s="68" t="s">
-        <v>312</v>
+        <v>287</v>
+      </c>
+      <c r="N71" s="42" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
@@ -4622,7 +4613,7 @@
         <v>148</v>
       </c>
       <c r="F72" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G72" s="20" t="s">
         <v>19</v>
@@ -4637,10 +4628,10 @@
       <c r="K72" s="33"/>
       <c r="L72" s="20"/>
       <c r="M72" s="20" t="s">
-        <v>290</v>
-      </c>
-      <c r="N72" s="68" t="s">
-        <v>312</v>
+        <v>287</v>
+      </c>
+      <c r="N72" s="42" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
@@ -4651,7 +4642,7 @@
         <v>146</v>
       </c>
       <c r="F73" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G73" s="20" t="s">
         <v>19</v>
@@ -4666,10 +4657,10 @@
       <c r="K73" s="33"/>
       <c r="L73" s="20"/>
       <c r="M73" s="20" t="s">
-        <v>290</v>
-      </c>
-      <c r="N73" s="68" t="s">
-        <v>312</v>
+        <v>287</v>
+      </c>
+      <c r="N73" s="42" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
@@ -4680,7 +4671,7 @@
         <v>144</v>
       </c>
       <c r="F74" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G74" s="20" t="s">
         <v>19</v>
@@ -4695,10 +4686,10 @@
       <c r="K74" s="33"/>
       <c r="L74" s="20"/>
       <c r="M74" s="20" t="s">
-        <v>289</v>
-      </c>
-      <c r="N74" s="68" t="s">
-        <v>312</v>
+        <v>286</v>
+      </c>
+      <c r="N74" s="42" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
@@ -4709,7 +4700,7 @@
         <v>142</v>
       </c>
       <c r="F75" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G75" s="20" t="s">
         <v>19</v>
@@ -4721,10 +4712,10 @@
       <c r="K75" s="33"/>
       <c r="L75" s="20"/>
       <c r="M75" s="20" t="s">
-        <v>288</v>
-      </c>
-      <c r="N75" s="68" t="s">
-        <v>311</v>
+        <v>285</v>
+      </c>
+      <c r="N75" s="42" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
@@ -4735,10 +4726,10 @@
         <v>140</v>
       </c>
       <c r="E76" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F76" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G76" s="20" t="s">
         <v>19</v>
@@ -4753,10 +4744,10 @@
       <c r="K76" s="33"/>
       <c r="L76" s="20"/>
       <c r="M76" s="20" t="s">
-        <v>287</v>
-      </c>
-      <c r="N76" s="68" t="s">
-        <v>310</v>
+        <v>284</v>
+      </c>
+      <c r="N76" s="42" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
@@ -4767,7 +4758,7 @@
         <v>138</v>
       </c>
       <c r="F77" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G77" s="20" t="s">
         <v>19</v>
@@ -4782,10 +4773,10 @@
       <c r="K77" s="33"/>
       <c r="L77" s="20"/>
       <c r="M77" s="20" t="s">
-        <v>286</v>
-      </c>
-      <c r="N77" s="68" t="s">
-        <v>310</v>
+        <v>283</v>
+      </c>
+      <c r="N77" s="42" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
@@ -4796,10 +4787,10 @@
         <v>136</v>
       </c>
       <c r="D78" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F78" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G78" s="20" t="s">
         <v>19</v>
@@ -4811,10 +4802,10 @@
       <c r="K78" s="33"/>
       <c r="L78" s="20"/>
       <c r="M78" s="20" t="s">
-        <v>276</v>
-      </c>
-      <c r="N78" s="68" t="s">
-        <v>309</v>
+        <v>273</v>
+      </c>
+      <c r="N78" s="42" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
@@ -4825,7 +4816,7 @@
         <v>134</v>
       </c>
       <c r="F79" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G79" s="20" t="s">
         <v>19</v>
@@ -4840,10 +4831,10 @@
       <c r="K79" s="33"/>
       <c r="L79" s="20"/>
       <c r="M79" s="20" t="s">
-        <v>285</v>
-      </c>
-      <c r="N79" s="68" t="s">
-        <v>308</v>
+        <v>282</v>
+      </c>
+      <c r="N79" s="42" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
@@ -4857,10 +4848,10 @@
         <v>126</v>
       </c>
       <c r="D80" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F80" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G80" s="20" t="s">
         <v>19</v>
@@ -4875,10 +4866,10 @@
       <c r="K80" s="33"/>
       <c r="L80" s="20"/>
       <c r="M80" s="20" t="s">
-        <v>284</v>
-      </c>
-      <c r="N80" s="68" t="s">
-        <v>307</v>
+        <v>281</v>
+      </c>
+      <c r="N80" s="42" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.2">
@@ -4892,10 +4883,10 @@
         <v>126</v>
       </c>
       <c r="D81" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F81" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G81" s="20" t="s">
         <v>19</v>
@@ -4910,10 +4901,10 @@
       <c r="K81" s="33"/>
       <c r="L81" s="20"/>
       <c r="M81" s="20" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="N81" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
@@ -4927,10 +4918,10 @@
         <v>126</v>
       </c>
       <c r="D82" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F82" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G82" s="20" t="s">
         <v>19</v>
@@ -4945,10 +4936,10 @@
       <c r="K82" s="33"/>
       <c r="L82" s="20"/>
       <c r="M82" s="20" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="N82" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
@@ -4962,10 +4953,10 @@
         <v>126</v>
       </c>
       <c r="D83" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F83" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G83" s="20" t="s">
         <v>19</v>
@@ -4980,10 +4971,10 @@
       <c r="K83" s="33"/>
       <c r="L83" s="20"/>
       <c r="M83" s="20" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="N83" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
@@ -4997,10 +4988,10 @@
         <v>121</v>
       </c>
       <c r="D84" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F84" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G84" s="20" t="s">
         <v>19</v>
@@ -5015,10 +5006,10 @@
       <c r="K84" s="33"/>
       <c r="L84" s="20"/>
       <c r="M84" s="20" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="N84" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.2">
@@ -5032,10 +5023,10 @@
         <v>121</v>
       </c>
       <c r="D85" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F85" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G85" s="20" t="s">
         <v>19</v>
@@ -5050,10 +5041,10 @@
       <c r="K85" s="33"/>
       <c r="L85" s="20"/>
       <c r="M85" s="20" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="N85" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
@@ -5067,10 +5058,10 @@
         <v>118</v>
       </c>
       <c r="D86" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F86" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G86" s="20" t="s">
         <v>19</v>
@@ -5085,27 +5076,27 @@
       <c r="K86" s="33"/>
       <c r="L86" s="20"/>
       <c r="M86" s="20" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="N86" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="B87" s="65" t="s">
+      <c r="B87" s="39" t="s">
         <v>116</v>
       </c>
       <c r="C87" t="s">
         <v>115</v>
       </c>
       <c r="D87" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F87" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G87" s="20" t="s">
         <v>19</v>
@@ -5120,10 +5111,10 @@
       <c r="K87" s="33"/>
       <c r="L87" s="20"/>
       <c r="M87" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="N87" s="68" t="s">
-        <v>305</v>
+        <v>280</v>
+      </c>
+      <c r="N87" s="42" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.2">
@@ -5134,10 +5125,10 @@
         <v>113</v>
       </c>
       <c r="D88" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F88" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G88" s="20" t="s">
         <v>19</v>
@@ -5149,10 +5140,10 @@
       <c r="K88" s="33"/>
       <c r="L88" s="20"/>
       <c r="M88" s="20" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="N88" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
@@ -5163,7 +5154,7 @@
         <v>111</v>
       </c>
       <c r="F89" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G89" s="20" t="s">
         <v>19</v>
@@ -5175,10 +5166,10 @@
       <c r="K89" s="33"/>
       <c r="L89" s="20"/>
       <c r="M89" s="20" t="s">
-        <v>281</v>
-      </c>
-      <c r="N89" s="68" t="s">
-        <v>303</v>
+        <v>278</v>
+      </c>
+      <c r="N89" s="42" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.2">
@@ -5192,10 +5183,10 @@
         <v>100</v>
       </c>
       <c r="E90" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F90" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G90" s="20" t="s">
         <v>19</v>
@@ -5210,10 +5201,10 @@
       <c r="K90" s="33"/>
       <c r="L90" s="20"/>
       <c r="M90" s="20" t="s">
-        <v>280</v>
-      </c>
-      <c r="N90" s="68" t="s">
-        <v>302</v>
+        <v>277</v>
+      </c>
+      <c r="N90" s="42" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.2">
@@ -5227,10 +5218,10 @@
         <v>100</v>
       </c>
       <c r="E91" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F91" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G91" s="20" t="s">
         <v>19</v>
@@ -5245,10 +5236,10 @@
       <c r="K91" s="33"/>
       <c r="L91" s="20"/>
       <c r="M91" s="20" t="s">
-        <v>280</v>
-      </c>
-      <c r="N91" s="68" t="s">
-        <v>302</v>
+        <v>277</v>
+      </c>
+      <c r="N91" s="42" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.2">
@@ -5259,7 +5250,7 @@
         <v>107</v>
       </c>
       <c r="F92" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G92" s="20" t="s">
         <v>19</v>
@@ -5271,10 +5262,10 @@
       <c r="K92" s="33"/>
       <c r="L92" s="20"/>
       <c r="M92" s="20" t="s">
-        <v>280</v>
-      </c>
-      <c r="N92" s="68" t="s">
-        <v>302</v>
+        <v>277</v>
+      </c>
+      <c r="N92" s="42" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.2">
@@ -5285,7 +5276,7 @@
         <v>105</v>
       </c>
       <c r="F93" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G93" s="20" t="s">
         <v>19</v>
@@ -5300,10 +5291,10 @@
       <c r="K93" s="33"/>
       <c r="L93" s="20"/>
       <c r="M93" s="20" t="s">
-        <v>279</v>
-      </c>
-      <c r="N93" s="68" t="s">
-        <v>301</v>
+        <v>276</v>
+      </c>
+      <c r="N93" s="42" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.2">
@@ -5314,7 +5305,7 @@
         <v>103</v>
       </c>
       <c r="F94" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G94" s="20" t="s">
         <v>19</v>
@@ -5329,10 +5320,10 @@
       <c r="K94" s="33"/>
       <c r="L94" s="20"/>
       <c r="M94" s="20" t="s">
-        <v>279</v>
-      </c>
-      <c r="N94" s="68" t="s">
-        <v>301</v>
+        <v>276</v>
+      </c>
+      <c r="N94" s="42" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.2">
@@ -5346,10 +5337,10 @@
         <v>100</v>
       </c>
       <c r="D95" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F95" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G95" s="20" t="s">
         <v>19</v>
@@ -5364,10 +5355,10 @@
       <c r="K95" s="33"/>
       <c r="L95" s="20"/>
       <c r="M95" s="20" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="N95" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.2">
@@ -5381,10 +5372,10 @@
         <v>97</v>
       </c>
       <c r="D96" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F96" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G96" s="20" t="s">
         <v>19</v>
@@ -5399,10 +5390,10 @@
       <c r="K96" s="33"/>
       <c r="L96" s="20"/>
       <c r="M96" s="20" t="s">
-        <v>277</v>
-      </c>
-      <c r="N96" s="68" t="s">
-        <v>299</v>
+        <v>274</v>
+      </c>
+      <c r="N96" s="42" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.2">
@@ -5416,10 +5407,10 @@
         <v>94</v>
       </c>
       <c r="D97" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F97" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G97" s="20" t="s">
         <v>19</v>
@@ -5434,10 +5425,10 @@
       <c r="K97" s="33"/>
       <c r="L97" s="20"/>
       <c r="M97" s="20" t="s">
-        <v>277</v>
-      </c>
-      <c r="N97" s="68" t="s">
-        <v>299</v>
+        <v>274</v>
+      </c>
+      <c r="N97" s="42" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.2">
@@ -5451,7 +5442,7 @@
         <v>87</v>
       </c>
       <c r="F98" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G98" s="20" t="s">
         <v>19</v>
@@ -5466,10 +5457,10 @@
       <c r="K98" s="33"/>
       <c r="L98" s="20"/>
       <c r="M98" s="20" t="s">
-        <v>276</v>
-      </c>
-      <c r="N98" s="68" t="s">
-        <v>298</v>
+        <v>273</v>
+      </c>
+      <c r="N98" s="42" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.2">
@@ -5483,7 +5474,7 @@
         <v>87</v>
       </c>
       <c r="F99" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G99" s="20" t="s">
         <v>19</v>
@@ -5498,10 +5489,10 @@
       <c r="K99" s="33"/>
       <c r="L99" s="20"/>
       <c r="M99" s="20" t="s">
-        <v>276</v>
-      </c>
-      <c r="N99" s="68" t="s">
-        <v>298</v>
+        <v>273</v>
+      </c>
+      <c r="N99" s="42" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.2">
@@ -5515,7 +5506,7 @@
         <v>87</v>
       </c>
       <c r="F100" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G100" s="20" t="s">
         <v>19</v>
@@ -5530,21 +5521,21 @@
       <c r="K100" s="33"/>
       <c r="L100" s="20"/>
       <c r="M100" s="20" t="s">
-        <v>276</v>
-      </c>
-      <c r="N100" s="68" t="s">
-        <v>298</v>
+        <v>273</v>
+      </c>
+      <c r="N100" s="42" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="B101" s="64" t="s">
+      <c r="B101" s="38" t="s">
         <v>85</v>
       </c>
       <c r="F101" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G101" s="20" t="s">
         <v>19</v>
@@ -5559,21 +5550,21 @@
       <c r="K101" s="33"/>
       <c r="L101" s="20"/>
       <c r="M101" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N101" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="B102" s="64" t="s">
+      <c r="B102" s="38" t="s">
         <v>83</v>
       </c>
       <c r="F102" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G102" s="20" t="s">
         <v>19</v>
@@ -5588,21 +5579,21 @@
       <c r="K102" s="33"/>
       <c r="L102" s="20"/>
       <c r="M102" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N102" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="B103" s="64" t="s">
+      <c r="B103" s="38" t="s">
         <v>81</v>
       </c>
       <c r="F103" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G103" s="20" t="s">
         <v>19</v>
@@ -5617,21 +5608,21 @@
       <c r="K103" s="33"/>
       <c r="L103" s="20"/>
       <c r="M103" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N103" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="B104" s="64" t="s">
+      <c r="B104" s="38" t="s">
         <v>79</v>
       </c>
       <c r="F104" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G104" s="20" t="s">
         <v>19</v>
@@ -5646,21 +5637,21 @@
       <c r="K104" s="33"/>
       <c r="L104" s="20"/>
       <c r="M104" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N104" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="B105" s="64" t="s">
+      <c r="B105" s="38" t="s">
         <v>77</v>
       </c>
       <c r="F105" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G105" s="20" t="s">
         <v>19</v>
@@ -5675,21 +5666,21 @@
       <c r="K105" s="33"/>
       <c r="L105" s="20"/>
       <c r="M105" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N105" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="B106" s="64" t="s">
+      <c r="B106" s="38" t="s">
         <v>75</v>
       </c>
       <c r="F106" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G106" s="20" t="s">
         <v>19</v>
@@ -5704,21 +5695,21 @@
       <c r="K106" s="33"/>
       <c r="L106" s="20"/>
       <c r="M106" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N106" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="B107" s="64" t="s">
+      <c r="B107" s="38" t="s">
         <v>73</v>
       </c>
       <c r="F107" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G107" s="20" t="s">
         <v>19</v>
@@ -5733,21 +5724,21 @@
       <c r="K107" s="33"/>
       <c r="L107" s="20"/>
       <c r="M107" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N107" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A108" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="B108" s="64" t="s">
+      <c r="B108" s="38" t="s">
         <v>71</v>
       </c>
       <c r="F108" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G108" s="20" t="s">
         <v>19</v>
@@ -5762,24 +5753,24 @@
       <c r="K108" s="33"/>
       <c r="L108" s="20"/>
       <c r="M108" s="20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N108" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A109" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="B109" s="64" t="s">
+      <c r="B109" s="38" t="s">
         <v>69</v>
       </c>
       <c r="C109" t="s">
         <v>68</v>
       </c>
       <c r="F109" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G109" s="20" t="s">
         <v>19</v>
@@ -5794,24 +5785,24 @@
       <c r="K109" s="33"/>
       <c r="L109" s="20"/>
       <c r="M109" s="20" t="s">
-        <v>275</v>
-      </c>
-      <c r="N109" s="68" t="s">
-        <v>296</v>
+        <v>272</v>
+      </c>
+      <c r="N109" s="42" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A110" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="B110" s="64" t="s">
+      <c r="B110" s="38" t="s">
         <v>66</v>
       </c>
       <c r="C110" t="s">
         <v>61</v>
       </c>
       <c r="F110" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G110" s="20" t="s">
         <v>19</v>
@@ -5826,24 +5817,24 @@
       <c r="K110" s="33"/>
       <c r="L110" s="20"/>
       <c r="M110" s="20" t="s">
-        <v>275</v>
-      </c>
-      <c r="N110" s="68" t="s">
-        <v>296</v>
+        <v>272</v>
+      </c>
+      <c r="N110" s="42" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A111" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="B111" s="64" t="s">
+      <c r="B111" s="38" t="s">
         <v>64</v>
       </c>
       <c r="C111" t="s">
         <v>61</v>
       </c>
       <c r="F111" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G111" s="20" t="s">
         <v>19</v>
@@ -5858,17 +5849,17 @@
       <c r="K111" s="33"/>
       <c r="L111" s="20"/>
       <c r="M111" s="20" t="s">
-        <v>275</v>
-      </c>
-      <c r="N111" s="68" t="s">
-        <v>296</v>
+        <v>272</v>
+      </c>
+      <c r="N111" s="42" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A112" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="B112" s="64" t="s">
+      <c r="B112" s="38" t="s">
         <v>62</v>
       </c>
       <c r="C112" t="s">
@@ -5877,7 +5868,7 @@
       <c r="D112" s="34"/>
       <c r="E112" s="20"/>
       <c r="F112" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G112" s="20" t="s">
         <v>19</v>
@@ -5892,10 +5883,10 @@
       <c r="K112" s="33"/>
       <c r="L112" s="20"/>
       <c r="M112" s="20" t="s">
-        <v>275</v>
-      </c>
-      <c r="N112" s="68" t="s">
-        <v>296</v>
+        <v>272</v>
+      </c>
+      <c r="N112" s="42" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
@@ -10519,6 +10510,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="P8:T8"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="H5:H6"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="B8:E8"/>
@@ -10533,11 +10529,6 @@
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="L5:L6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="P8:T8"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
- added some additional units and comments to Hui's data
</commit_message>
<xml_diff>
--- a/HuiSun_FractureToughnessData_Jan2022_AdamFix.xlsx
+++ b/HuiSun_FractureToughnessData_Jan2022_AdamFix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-guest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785A0057-79F8-5D40-A59E-AE340C19104E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED95FD2A-4A58-5A4D-A256-9AC1371A8D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="760" windowWidth="34560" windowHeight="20240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="316">
   <si>
     <t>Name:</t>
   </si>
@@ -603,73 +603,37 @@
     <t>BCC+HCP</t>
   </si>
   <si>
-    <t>Ti86.2 Al10.2 V3.18</t>
-  </si>
-  <si>
     <t>51</t>
   </si>
   <si>
-    <t>Ti86.2 Al10.2 V3.17</t>
-  </si>
-  <si>
     <t>50</t>
   </si>
   <si>
-    <t>Ti86.2 Al10.2 V3.16</t>
-  </si>
-  <si>
     <t>49</t>
   </si>
   <si>
-    <t>Ti86.2 Al10.2 V3.15</t>
-  </si>
-  <si>
     <t>48</t>
   </si>
   <si>
-    <t>Ti86.2 Al10.2 V3.14</t>
-  </si>
-  <si>
     <t>47</t>
   </si>
   <si>
-    <t>Ti86.2 Al10.2 V3.13</t>
-  </si>
-  <si>
     <t>46</t>
   </si>
   <si>
-    <t>Ti86.2 Al10.2 V3.12</t>
-  </si>
-  <si>
     <t>45</t>
   </si>
   <si>
-    <t>Ti86.2 Al10.2 V3.11</t>
-  </si>
-  <si>
     <t>44</t>
   </si>
   <si>
-    <t>Ti86.2 Al10.2 V3.10</t>
-  </si>
-  <si>
     <t>43</t>
   </si>
   <si>
-    <t>Ti86.2 Al10.2 V3.9</t>
-  </si>
-  <si>
     <t>42</t>
   </si>
   <si>
-    <t>Ti86.2 Al10.2 V3.8</t>
-  </si>
-  <si>
     <t>41</t>
-  </si>
-  <si>
-    <t>Ti86.2 Al10.2 V3.7</t>
   </si>
   <si>
     <t>40</t>
@@ -949,12 +913,6 @@
     <t>Spheroidal BCC W in ductile FCC Ni-Fe-W solid solution</t>
   </si>
   <si>
-    <t>Bi-crystal</t>
-  </si>
-  <si>
-    <t>Single Crystal</t>
-  </si>
-  <si>
     <t>fracture toughness</t>
   </si>
   <si>
@@ -1112,6 +1070,30 @@
   </si>
   <si>
     <t>Data originally fetched by Hui; heavily edited and re-uploaded by Adam in Jan2022; additional bugfixing in Nov 2024</t>
+  </si>
+  <si>
+    <t>Pa m^0.5</t>
+  </si>
+  <si>
+    <t>nanoindentation</t>
+  </si>
+  <si>
+    <t>K test</t>
+  </si>
+  <si>
+    <t>J-R curve on CT</t>
+  </si>
+  <si>
+    <t>bending notched micro-cantilever</t>
+  </si>
+  <si>
+    <t>from a review paper</t>
+  </si>
+  <si>
+    <t>Single Crystal; from a review paper</t>
+  </si>
+  <si>
+    <t>Bi-crystal; from a review paper</t>
   </si>
 </sst>
 </file>
@@ -2187,8 +2169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2222,14 +2204,14 @@
         <v>0</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="D2" s="49" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="50"/>
       <c r="F2" s="45" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
       <c r="G2" s="45"/>
       <c r="H2" s="45"/>
@@ -2246,7 +2228,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="D3" s="51"/>
       <c r="E3" s="52"/>
@@ -2485,23 +2467,27 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
+      <c r="E10" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="F10" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G10" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="34"/>
+      <c r="H10" s="34" t="s">
+        <v>309</v>
+      </c>
       <c r="I10">
         <v>293</v>
       </c>
@@ -2509,34 +2495,40 @@
         <v>50900000</v>
       </c>
       <c r="K10" s="33"/>
-      <c r="L10" s="20"/>
+      <c r="L10" s="20" t="s">
+        <v>308</v>
+      </c>
       <c r="M10" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N10" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="O10" s="20"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="C11" s="20" t="s">
         <v>100</v>
       </c>
       <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
+      <c r="E11" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="F11" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G11" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="34"/>
+      <c r="H11" s="34" t="s">
+        <v>309</v>
+      </c>
       <c r="I11">
         <v>293</v>
       </c>
@@ -2544,34 +2536,40 @@
         <v>7600000</v>
       </c>
       <c r="K11" s="33"/>
-      <c r="L11" s="20"/>
+      <c r="L11" s="20" t="s">
+        <v>308</v>
+      </c>
       <c r="M11" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N11" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="O11" s="20"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="C12" s="20" t="s">
         <v>100</v>
       </c>
       <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
+      <c r="E12" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="F12" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G12" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H12" s="34"/>
+      <c r="H12" s="34" t="s">
+        <v>310</v>
+      </c>
       <c r="I12">
         <v>293</v>
       </c>
@@ -2579,34 +2577,40 @@
         <v>5600000</v>
       </c>
       <c r="K12" s="33"/>
-      <c r="L12" s="20"/>
+      <c r="L12" s="20" t="s">
+        <v>308</v>
+      </c>
       <c r="M12" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N12" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="O12" s="21"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="C13" s="20" t="s">
         <v>121</v>
       </c>
       <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
+      <c r="E13" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="F13" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G13" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="34"/>
+      <c r="H13" s="34" t="s">
+        <v>311</v>
+      </c>
       <c r="I13">
         <v>77</v>
       </c>
@@ -2614,34 +2618,40 @@
         <v>219000000</v>
       </c>
       <c r="K13" s="33"/>
-      <c r="L13" s="20"/>
+      <c r="L13" s="20" t="s">
+        <v>308</v>
+      </c>
       <c r="M13" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N13" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="O13" s="20"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="C14" s="20" t="s">
         <v>121</v>
       </c>
       <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
+      <c r="E14" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="F14" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H14" s="34"/>
+      <c r="H14" s="34" t="s">
+        <v>311</v>
+      </c>
       <c r="I14">
         <v>200</v>
       </c>
@@ -2649,34 +2659,40 @@
         <v>221000000</v>
       </c>
       <c r="K14" s="33"/>
-      <c r="L14" s="20"/>
+      <c r="L14" s="20" t="s">
+        <v>308</v>
+      </c>
       <c r="M14" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N14" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="O14" s="20"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>121</v>
       </c>
       <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
+      <c r="E15" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="F15" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G15" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H15" s="34"/>
+      <c r="H15" s="34" t="s">
+        <v>311</v>
+      </c>
       <c r="I15">
         <v>293</v>
       </c>
@@ -2684,34 +2700,40 @@
         <v>217000000</v>
       </c>
       <c r="K15" s="33"/>
-      <c r="L15" s="20"/>
+      <c r="L15" s="20" t="s">
+        <v>308</v>
+      </c>
       <c r="M15" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N15" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="O15" s="20"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
+      <c r="E16" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="F16" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G16" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H16" s="34"/>
+      <c r="H16" s="34" t="s">
+        <v>310</v>
+      </c>
       <c r="I16">
         <v>293</v>
       </c>
@@ -2719,32 +2741,39 @@
         <v>42500000</v>
       </c>
       <c r="K16" s="33"/>
-      <c r="L16" s="20"/>
+      <c r="L16" s="20" t="s">
+        <v>308</v>
+      </c>
       <c r="M16" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N16" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="O16" s="20"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>227</v>
+        <v>215</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>313</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G17" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H17" s="34"/>
+      <c r="H17" s="34" t="s">
+        <v>310</v>
+      </c>
       <c r="I17" s="41">
         <v>473</v>
       </c>
@@ -2752,31 +2781,38 @@
         <v>46500000</v>
       </c>
       <c r="K17" s="33"/>
-      <c r="L17" s="20"/>
+      <c r="L17" s="20" t="s">
+        <v>308</v>
+      </c>
       <c r="M17" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N17" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>227</v>
+        <v>215</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>313</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G18" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="34"/>
+      <c r="H18" s="34" t="s">
+        <v>310</v>
+      </c>
       <c r="I18">
         <v>293</v>
       </c>
@@ -2784,31 +2820,38 @@
         <v>33500000</v>
       </c>
       <c r="K18" s="33"/>
-      <c r="L18" s="20"/>
+      <c r="L18" s="20" t="s">
+        <v>308</v>
+      </c>
       <c r="M18" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N18" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="C19" s="20" t="s">
         <v>100</v>
       </c>
+      <c r="E19" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="F19" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G19" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H19" s="34"/>
+      <c r="H19" s="34" t="s">
+        <v>310</v>
+      </c>
       <c r="I19">
         <v>293</v>
       </c>
@@ -2816,31 +2859,38 @@
         <v>9000000</v>
       </c>
       <c r="K19" s="33"/>
-      <c r="L19" s="20"/>
+      <c r="L19" s="20" t="s">
+        <v>308</v>
+      </c>
       <c r="M19" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N19" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>227</v>
+        <v>215</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>313</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G20" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H20" s="34"/>
+      <c r="H20" s="34" t="s">
+        <v>310</v>
+      </c>
       <c r="I20">
         <v>293</v>
       </c>
@@ -2848,31 +2898,38 @@
         <v>11000000</v>
       </c>
       <c r="K20" s="33"/>
-      <c r="L20" s="20"/>
+      <c r="L20" s="20" t="s">
+        <v>308</v>
+      </c>
       <c r="M20" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N20" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>121</v>
       </c>
+      <c r="E21" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="F21" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G21" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H21" s="34"/>
+      <c r="H21" s="34" t="s">
+        <v>310</v>
+      </c>
       <c r="I21">
         <v>293</v>
       </c>
@@ -2880,31 +2937,38 @@
         <v>53000000</v>
       </c>
       <c r="K21" s="33"/>
-      <c r="L21" s="20"/>
+      <c r="L21" s="20" t="s">
+        <v>308</v>
+      </c>
       <c r="M21" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N21" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="C22" s="20" t="s">
         <v>121</v>
       </c>
+      <c r="E22" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="F22" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G22" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H22" s="34"/>
+      <c r="H22" s="34" t="s">
+        <v>311</v>
+      </c>
       <c r="I22">
         <v>77</v>
       </c>
@@ -2912,31 +2976,38 @@
         <v>273300000</v>
       </c>
       <c r="K22" s="33"/>
-      <c r="L22" s="20"/>
+      <c r="L22" s="20" t="s">
+        <v>308</v>
+      </c>
       <c r="M22" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N22" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="C23" s="20" t="s">
         <v>121</v>
       </c>
+      <c r="E23" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="F23" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G23" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H23" s="34"/>
+      <c r="H23" s="34" t="s">
+        <v>311</v>
+      </c>
       <c r="I23">
         <v>198</v>
       </c>
@@ -2944,31 +3015,38 @@
         <v>265200000</v>
       </c>
       <c r="K23" s="33"/>
-      <c r="L23" s="20"/>
+      <c r="L23" s="20" t="s">
+        <v>308</v>
+      </c>
       <c r="M23" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N23" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="C24" s="20" t="s">
         <v>121</v>
       </c>
+      <c r="E24" s="20" t="s">
+        <v>313</v>
+      </c>
       <c r="F24" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G24" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H24" s="34"/>
+      <c r="H24" s="34" t="s">
+        <v>311</v>
+      </c>
       <c r="I24">
         <v>293</v>
       </c>
@@ -2976,34 +3054,38 @@
         <v>207700000</v>
       </c>
       <c r="K24" s="33"/>
-      <c r="L24" s="20"/>
+      <c r="L24" s="20" t="s">
+        <v>308</v>
+      </c>
       <c r="M24" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N24" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="C25" s="20" t="s">
         <v>100</v>
       </c>
       <c r="E25" t="s">
-        <v>268</v>
+        <v>314</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G25" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H25" s="34"/>
+      <c r="H25" s="34" t="s">
+        <v>312</v>
+      </c>
       <c r="I25">
         <v>298</v>
       </c>
@@ -3011,34 +3093,38 @@
         <v>1600000</v>
       </c>
       <c r="K25" s="33"/>
-      <c r="L25" s="20"/>
+      <c r="L25" s="20" t="s">
+        <v>308</v>
+      </c>
       <c r="M25" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N25" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="E26" t="s">
-        <v>267</v>
+        <v>315</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G26" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H26" s="34"/>
+      <c r="H26" s="34" t="s">
+        <v>312</v>
+      </c>
       <c r="I26">
         <v>298</v>
       </c>
@@ -3046,26 +3132,31 @@
         <v>200000</v>
       </c>
       <c r="K26" s="33"/>
-      <c r="L26" s="20"/>
+      <c r="L26" s="20" t="s">
+        <v>308</v>
+      </c>
       <c r="M26" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N26" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="C27" s="20" t="s">
         <v>100</v>
       </c>
+      <c r="E27" t="s">
+        <v>313</v>
+      </c>
       <c r="F27" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G27" s="20" t="s">
         <v>19</v>
@@ -3080,24 +3171,27 @@
       <c r="K27" s="33"/>
       <c r="L27" s="20"/>
       <c r="M27" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N27" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="C28" s="20" t="s">
         <v>100</v>
       </c>
+      <c r="E28" t="s">
+        <v>313</v>
+      </c>
       <c r="F28" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G28" s="20" t="s">
         <v>19</v>
@@ -3112,24 +3206,27 @@
       <c r="K28" s="33"/>
       <c r="L28" s="20"/>
       <c r="M28" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N28" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="C29" s="20" t="s">
         <v>100</v>
       </c>
+      <c r="E29" t="s">
+        <v>313</v>
+      </c>
       <c r="F29" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G29" s="20" t="s">
         <v>19</v>
@@ -3144,24 +3241,27 @@
       <c r="K29" s="33"/>
       <c r="L29" s="20"/>
       <c r="M29" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N29" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="C30" s="20" t="s">
         <v>100</v>
       </c>
+      <c r="E30" t="s">
+        <v>313</v>
+      </c>
       <c r="F30" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G30" s="20" t="s">
         <v>19</v>
@@ -3176,24 +3276,24 @@
       <c r="K30" s="33"/>
       <c r="L30" s="20"/>
       <c r="M30" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N30" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="C31" s="20" t="s">
         <v>121</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G31" s="20" t="s">
         <v>19</v>
@@ -3208,24 +3308,24 @@
       <c r="K31" s="33"/>
       <c r="L31" s="20"/>
       <c r="M31" s="20" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="N31" s="43" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="C32" s="20" t="s">
         <v>121</v>
       </c>
       <c r="F32" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G32" s="20" t="s">
         <v>19</v>
@@ -3240,24 +3340,24 @@
       <c r="K32" s="33"/>
       <c r="L32" s="20"/>
       <c r="M32" s="20" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="N32" s="43" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="20" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="C33" s="20" t="s">
         <v>100</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G33" s="20" t="s">
         <v>19</v>
@@ -3272,24 +3372,24 @@
       <c r="K33" s="33"/>
       <c r="L33" s="20"/>
       <c r="M33" s="20" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
       <c r="N33" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="20" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="C34" s="40" t="s">
         <v>118</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G34" s="20" t="s">
         <v>19</v>
@@ -3304,24 +3404,24 @@
       <c r="K34" s="33"/>
       <c r="L34" s="20"/>
       <c r="M34" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N34" s="42" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="C35" s="40" t="s">
         <v>118</v>
       </c>
       <c r="F35" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G35" s="20" t="s">
         <v>19</v>
@@ -3336,24 +3436,24 @@
       <c r="K35" s="33"/>
       <c r="L35" s="20"/>
       <c r="M35" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N35" s="42" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="C36" s="40" t="s">
         <v>118</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G36" s="20" t="s">
         <v>19</v>
@@ -3368,27 +3468,27 @@
       <c r="K36" s="33"/>
       <c r="L36" s="20"/>
       <c r="M36" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N36" s="42" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="20" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="C37" s="40" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G37" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="H37" s="34"/>
       <c r="J37">
@@ -3397,24 +3497,24 @@
       <c r="K37" s="33"/>
       <c r="L37" s="20"/>
       <c r="M37" s="20" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="N37" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="20" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="C38" s="40" t="s">
         <v>100</v>
       </c>
       <c r="F38" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G38" s="20" t="s">
         <v>19</v>
@@ -3429,24 +3529,24 @@
       <c r="K38" s="33"/>
       <c r="L38" s="20"/>
       <c r="M38" s="20" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="N38" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="20" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="C39" s="40" t="s">
         <v>100</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G39" s="20" t="s">
         <v>19</v>
@@ -3461,15 +3561,15 @@
       <c r="K39" s="33"/>
       <c r="L39" s="20"/>
       <c r="M39" s="20" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="N39" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="20" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="B40" s="20" t="s">
         <v>107</v>
@@ -3478,7 +3578,7 @@
         <v>100</v>
       </c>
       <c r="F40" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G40" s="20" t="s">
         <v>19</v>
@@ -3493,30 +3593,30 @@
       <c r="K40" s="33"/>
       <c r="L40" s="20"/>
       <c r="M40" s="20" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="N40" s="42" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="20" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="C41" s="40" t="s">
         <v>126</v>
       </c>
       <c r="D41" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="E41" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="F41" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G41" s="20" t="s">
         <v>19</v>
@@ -3531,30 +3631,30 @@
       <c r="K41" s="33"/>
       <c r="L41" s="20"/>
       <c r="M41" s="20" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="N41" s="42" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="20" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="C42" s="40" t="s">
         <v>126</v>
       </c>
       <c r="D42" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="E42" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="F42" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G42" s="20" t="s">
         <v>19</v>
@@ -3569,30 +3669,30 @@
       <c r="K42" s="33"/>
       <c r="L42" s="20"/>
       <c r="M42" s="20" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="N42" s="42" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="20" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="C43" s="40" t="s">
         <v>126</v>
       </c>
       <c r="D43" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="E43" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G43" s="20" t="s">
         <v>19</v>
@@ -3607,30 +3707,30 @@
       <c r="K43" s="33"/>
       <c r="L43" s="20"/>
       <c r="M43" s="20" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="N43" s="42" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="20" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="C44" s="40" t="s">
         <v>126</v>
       </c>
       <c r="D44" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="E44" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="F44" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G44" s="20" t="s">
         <v>19</v>
@@ -3645,30 +3745,30 @@
       <c r="K44" s="33"/>
       <c r="L44" s="20"/>
       <c r="M44" s="20" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="N44" s="42" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="20" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="C45" s="40" t="s">
         <v>126</v>
       </c>
       <c r="D45" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="E45" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="F45" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G45" s="20" t="s">
         <v>19</v>
@@ -3683,30 +3783,30 @@
       <c r="K45" s="33"/>
       <c r="L45" s="20"/>
       <c r="M45" s="20" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="N45" s="42" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="20" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="C46" s="40" t="s">
         <v>126</v>
       </c>
       <c r="D46" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="E46" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="F46" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G46" s="20" t="s">
         <v>19</v>
@@ -3721,30 +3821,30 @@
       <c r="K46" s="33"/>
       <c r="L46" s="20"/>
       <c r="M46" s="20" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="N46" s="42" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="20" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="B47" s="20" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="C47" s="40" t="s">
         <v>126</v>
       </c>
       <c r="D47" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="E47" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="F47" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G47" s="20" t="s">
         <v>19</v>
@@ -3759,30 +3859,30 @@
       <c r="K47" s="33"/>
       <c r="L47" s="20"/>
       <c r="M47" s="20" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="N47" s="42" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="20" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="B48" s="20" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="C48" s="40" t="s">
         <v>126</v>
       </c>
       <c r="D48" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="E48" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="F48" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G48" s="20" t="s">
         <v>19</v>
@@ -3797,30 +3897,30 @@
       <c r="K48" s="33"/>
       <c r="L48" s="20"/>
       <c r="M48" s="20" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="N48" s="42" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="20" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="B49" s="20" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="C49" s="40" t="s">
         <v>126</v>
       </c>
       <c r="D49" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="E49" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="F49" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G49" s="20" t="s">
         <v>19</v>
@@ -3835,30 +3935,30 @@
       <c r="K49" s="33"/>
       <c r="L49" s="20"/>
       <c r="M49" s="20" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="N49" s="42" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="20" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="B50" s="20" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="C50" s="40" t="s">
         <v>126</v>
       </c>
       <c r="D50" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="E50" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="F50" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G50" s="20" t="s">
         <v>19</v>
@@ -3873,30 +3973,30 @@
       <c r="K50" s="33"/>
       <c r="L50" s="20"/>
       <c r="M50" s="20" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="N50" s="42" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="20" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="B51" s="20" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="C51" s="40" t="s">
         <v>126</v>
       </c>
       <c r="D51" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="E51" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="F51" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G51" s="20" t="s">
         <v>19</v>
@@ -3911,30 +4011,30 @@
       <c r="K51" s="33"/>
       <c r="L51" s="20"/>
       <c r="M51" s="20" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="N51" s="42" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="20" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="B52" s="20" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="C52" s="40" t="s">
         <v>126</v>
       </c>
       <c r="D52" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="E52" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="F52" s="20" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="G52" s="20" t="s">
         <v>19</v>
@@ -3949,30 +4049,30 @@
       <c r="K52" s="33"/>
       <c r="L52" s="20"/>
       <c r="M52" s="20" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="N52" s="42" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="53" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="20" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="B53" s="20" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="C53" s="40" t="s">
         <v>126</v>
       </c>
       <c r="D53" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="E53" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="F53" s="20" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="G53" s="20" t="s">
         <v>19</v>
@@ -3987,30 +4087,30 @@
       <c r="K53" s="33"/>
       <c r="L53" s="20"/>
       <c r="M53" s="20" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="N53" s="42" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="20" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="B54" s="20" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="C54" s="40" t="s">
         <v>126</v>
       </c>
       <c r="D54" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="E54" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="F54" s="20" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="G54" s="20" t="s">
         <v>19</v>
@@ -4025,30 +4125,30 @@
       <c r="K54" s="33"/>
       <c r="L54" s="20"/>
       <c r="M54" s="20" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="N54" s="42" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="55" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="20" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="B55" s="20" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="C55" s="40" t="s">
         <v>126</v>
       </c>
       <c r="D55" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="E55" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="F55" s="20" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="G55" s="20" t="s">
         <v>19</v>
@@ -4063,30 +4163,30 @@
       <c r="K55" s="33"/>
       <c r="L55" s="20"/>
       <c r="M55" s="20" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="N55" s="42" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="56" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="20" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="B56" s="20" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="C56" s="40" t="s">
         <v>157</v>
       </c>
       <c r="D56" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="E56" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="F56" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G56" s="20" t="s">
         <v>19</v>
@@ -4098,30 +4198,30 @@
       <c r="K56" s="33"/>
       <c r="L56" s="20"/>
       <c r="M56" s="20" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="N56" s="42" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="57" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="20" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="B57" s="20" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="C57" s="40" t="s">
         <v>157</v>
       </c>
       <c r="D57" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="E57" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="F57" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G57" s="20" t="s">
         <v>19</v>
@@ -4133,30 +4233,30 @@
       <c r="K57" s="33"/>
       <c r="L57" s="20"/>
       <c r="M57" s="20" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="N57" s="42" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="20" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="B58" s="20" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="C58" s="40" t="s">
         <v>157</v>
       </c>
       <c r="D58" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="E58" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="F58" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G58" s="20" t="s">
         <v>19</v>
@@ -4168,30 +4268,30 @@
       <c r="K58" s="33"/>
       <c r="L58" s="20"/>
       <c r="M58" s="20" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="N58" s="42" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="59" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="20" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="B59" s="20" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C59" s="40" t="s">
         <v>157</v>
       </c>
       <c r="D59" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="E59" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="F59" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G59" s="20" t="s">
         <v>19</v>
@@ -4203,30 +4303,30 @@
       <c r="K59" s="33"/>
       <c r="L59" s="20"/>
       <c r="M59" s="20" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="N59" s="42" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="60" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="20" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="B60" s="20" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C60" s="40" t="s">
         <v>157</v>
       </c>
       <c r="D60" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="E60" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="F60" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G60" s="20" t="s">
         <v>19</v>
@@ -4238,30 +4338,30 @@
       <c r="K60" s="33"/>
       <c r="L60" s="20"/>
       <c r="M60" s="20" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="N60" s="42" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="61" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="20" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="B61" s="20" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C61" s="40" t="s">
         <v>157</v>
       </c>
       <c r="D61" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="E61" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="F61" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G61" s="20" t="s">
         <v>19</v>
@@ -4273,15 +4373,15 @@
       <c r="K61" s="33"/>
       <c r="L61" s="20"/>
       <c r="M61" s="20" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="N61" s="42" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="62" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="20" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B62" s="20" t="s">
         <v>170</v>
@@ -4290,13 +4390,13 @@
         <v>157</v>
       </c>
       <c r="D62" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="E62" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="F62" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G62" s="20" t="s">
         <v>19</v>
@@ -4308,27 +4408,27 @@
       <c r="K62" s="33"/>
       <c r="L62" s="20"/>
       <c r="M62" s="20" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="N62" s="42" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="63" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="20" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B63" s="20" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C63" s="40" t="s">
         <v>157</v>
       </c>
       <c r="D63" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="F63" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G63" s="20" t="s">
         <v>19</v>
@@ -4340,27 +4440,27 @@
       <c r="K63" s="33"/>
       <c r="L63" s="20"/>
       <c r="M63" s="20" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="N63" s="42" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="64" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="20" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B64" s="20" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C64" s="40" t="s">
         <v>157</v>
       </c>
       <c r="D64" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="F64" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G64" s="20" t="s">
         <v>19</v>
@@ -4372,27 +4472,27 @@
       <c r="K64" s="33"/>
       <c r="L64" s="20"/>
       <c r="M64" s="20" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="N64" s="42" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="65" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="20" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B65" s="20" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="C65" s="40" t="s">
         <v>157</v>
       </c>
       <c r="D65" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="F65" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G65" s="20" t="s">
         <v>19</v>
@@ -4404,27 +4504,27 @@
       <c r="K65" s="33"/>
       <c r="L65" s="20"/>
       <c r="M65" s="20" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="N65" s="42" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="66" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="20" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B66" s="20" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="C66" s="40" t="s">
         <v>157</v>
       </c>
       <c r="D66" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="F66" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G66" s="20" t="s">
         <v>19</v>
@@ -4436,27 +4536,27 @@
       <c r="K66" s="33"/>
       <c r="L66" s="20"/>
       <c r="M66" s="20" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="N66" s="42" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="67" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="20" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B67" s="20" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="C67" s="40" t="s">
         <v>157</v>
       </c>
       <c r="D67" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="F67" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G67" s="20" t="s">
         <v>19</v>
@@ -4468,27 +4568,27 @@
       <c r="K67" s="33"/>
       <c r="L67" s="20"/>
       <c r="M67" s="20" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="N67" s="42" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="68" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B68" s="20" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="C68" s="40" t="s">
         <v>157</v>
       </c>
       <c r="D68" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="F68" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G68" s="20" t="s">
         <v>19</v>
@@ -4500,10 +4600,10 @@
       <c r="K68" s="33"/>
       <c r="L68" s="20"/>
       <c r="M68" s="20" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="N68" s="42" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
@@ -4517,10 +4617,10 @@
         <v>152</v>
       </c>
       <c r="D69" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="F69" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G69" s="20" t="s">
         <v>19</v>
@@ -4535,10 +4635,10 @@
       <c r="K69" s="33"/>
       <c r="L69" s="20"/>
       <c r="M69" s="20" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="N69" s="42" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
@@ -4552,10 +4652,10 @@
         <v>152</v>
       </c>
       <c r="D70" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="F70" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G70" s="20" t="s">
         <v>19</v>
@@ -4570,10 +4670,10 @@
       <c r="K70" s="33"/>
       <c r="L70" s="20"/>
       <c r="M70" s="20" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="N70" s="42" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
@@ -4584,7 +4684,7 @@
         <v>150</v>
       </c>
       <c r="F71" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G71" s="20" t="s">
         <v>19</v>
@@ -4599,10 +4699,10 @@
       <c r="K71" s="33"/>
       <c r="L71" s="20"/>
       <c r="M71" s="20" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="N71" s="42" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
@@ -4613,7 +4713,7 @@
         <v>148</v>
       </c>
       <c r="F72" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G72" s="20" t="s">
         <v>19</v>
@@ -4628,10 +4728,10 @@
       <c r="K72" s="33"/>
       <c r="L72" s="20"/>
       <c r="M72" s="20" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="N72" s="42" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
@@ -4642,7 +4742,7 @@
         <v>146</v>
       </c>
       <c r="F73" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G73" s="20" t="s">
         <v>19</v>
@@ -4657,10 +4757,10 @@
       <c r="K73" s="33"/>
       <c r="L73" s="20"/>
       <c r="M73" s="20" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="N73" s="42" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
@@ -4671,7 +4771,7 @@
         <v>144</v>
       </c>
       <c r="F74" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G74" s="20" t="s">
         <v>19</v>
@@ -4686,10 +4786,10 @@
       <c r="K74" s="33"/>
       <c r="L74" s="20"/>
       <c r="M74" s="20" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="N74" s="42" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
@@ -4700,7 +4800,7 @@
         <v>142</v>
       </c>
       <c r="F75" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G75" s="20" t="s">
         <v>19</v>
@@ -4712,10 +4812,10 @@
       <c r="K75" s="33"/>
       <c r="L75" s="20"/>
       <c r="M75" s="20" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="N75" s="42" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
@@ -4726,10 +4826,10 @@
         <v>140</v>
       </c>
       <c r="E76" t="s">
+        <v>243</v>
+      </c>
+      <c r="F76" s="20" t="s">
         <v>255</v>
-      </c>
-      <c r="F76" s="20" t="s">
-        <v>269</v>
       </c>
       <c r="G76" s="20" t="s">
         <v>19</v>
@@ -4744,10 +4844,10 @@
       <c r="K76" s="33"/>
       <c r="L76" s="20"/>
       <c r="M76" s="20" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="N76" s="42" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
@@ -4758,7 +4858,7 @@
         <v>138</v>
       </c>
       <c r="F77" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G77" s="20" t="s">
         <v>19</v>
@@ -4773,10 +4873,10 @@
       <c r="K77" s="33"/>
       <c r="L77" s="20"/>
       <c r="M77" s="20" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="N77" s="42" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
@@ -4787,10 +4887,10 @@
         <v>136</v>
       </c>
       <c r="D78" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="F78" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G78" s="20" t="s">
         <v>19</v>
@@ -4802,10 +4902,10 @@
       <c r="K78" s="33"/>
       <c r="L78" s="20"/>
       <c r="M78" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N78" s="42" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
@@ -4816,7 +4916,7 @@
         <v>134</v>
       </c>
       <c r="F79" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G79" s="20" t="s">
         <v>19</v>
@@ -4831,10 +4931,10 @@
       <c r="K79" s="33"/>
       <c r="L79" s="20"/>
       <c r="M79" s="20" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="N79" s="42" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
@@ -4848,10 +4948,10 @@
         <v>126</v>
       </c>
       <c r="D80" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="F80" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G80" s="20" t="s">
         <v>19</v>
@@ -4866,10 +4966,10 @@
       <c r="K80" s="33"/>
       <c r="L80" s="20"/>
       <c r="M80" s="20" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="N80" s="42" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.2">
@@ -4883,10 +4983,10 @@
         <v>126</v>
       </c>
       <c r="D81" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="F81" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G81" s="20" t="s">
         <v>19</v>
@@ -4901,10 +5001,10 @@
       <c r="K81" s="33"/>
       <c r="L81" s="20"/>
       <c r="M81" s="20" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="N81" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
@@ -4918,10 +5018,10 @@
         <v>126</v>
       </c>
       <c r="D82" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="F82" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G82" s="20" t="s">
         <v>19</v>
@@ -4936,10 +5036,10 @@
       <c r="K82" s="33"/>
       <c r="L82" s="20"/>
       <c r="M82" s="20" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="N82" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
@@ -4953,10 +5053,10 @@
         <v>126</v>
       </c>
       <c r="D83" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="F83" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G83" s="20" t="s">
         <v>19</v>
@@ -4971,10 +5071,10 @@
       <c r="K83" s="33"/>
       <c r="L83" s="20"/>
       <c r="M83" s="20" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="N83" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
@@ -4988,10 +5088,10 @@
         <v>121</v>
       </c>
       <c r="D84" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="F84" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G84" s="20" t="s">
         <v>19</v>
@@ -5006,10 +5106,10 @@
       <c r="K84" s="33"/>
       <c r="L84" s="20"/>
       <c r="M84" s="20" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="N84" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.2">
@@ -5023,10 +5123,10 @@
         <v>121</v>
       </c>
       <c r="D85" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="F85" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G85" s="20" t="s">
         <v>19</v>
@@ -5041,10 +5141,10 @@
       <c r="K85" s="33"/>
       <c r="L85" s="20"/>
       <c r="M85" s="20" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="N85" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
@@ -5058,10 +5158,10 @@
         <v>118</v>
       </c>
       <c r="D86" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="F86" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G86" s="20" t="s">
         <v>19</v>
@@ -5076,10 +5176,10 @@
       <c r="K86" s="33"/>
       <c r="L86" s="20"/>
       <c r="M86" s="20" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="N86" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.2">
@@ -5093,10 +5193,10 @@
         <v>115</v>
       </c>
       <c r="D87" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="F87" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G87" s="20" t="s">
         <v>19</v>
@@ -5111,10 +5211,10 @@
       <c r="K87" s="33"/>
       <c r="L87" s="20"/>
       <c r="M87" s="20" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="N87" s="42" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.2">
@@ -5125,10 +5225,10 @@
         <v>113</v>
       </c>
       <c r="D88" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="F88" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G88" s="20" t="s">
         <v>19</v>
@@ -5140,10 +5240,10 @@
       <c r="K88" s="33"/>
       <c r="L88" s="20"/>
       <c r="M88" s="20" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="N88" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
@@ -5154,7 +5254,7 @@
         <v>111</v>
       </c>
       <c r="F89" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G89" s="20" t="s">
         <v>19</v>
@@ -5166,10 +5266,10 @@
       <c r="K89" s="33"/>
       <c r="L89" s="20"/>
       <c r="M89" s="20" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="N89" s="42" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.2">
@@ -5183,10 +5283,10 @@
         <v>100</v>
       </c>
       <c r="E90" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="F90" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G90" s="20" t="s">
         <v>19</v>
@@ -5201,10 +5301,10 @@
       <c r="K90" s="33"/>
       <c r="L90" s="20"/>
       <c r="M90" s="20" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="N90" s="42" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.2">
@@ -5218,10 +5318,10 @@
         <v>100</v>
       </c>
       <c r="E91" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="F91" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G91" s="20" t="s">
         <v>19</v>
@@ -5236,10 +5336,10 @@
       <c r="K91" s="33"/>
       <c r="L91" s="20"/>
       <c r="M91" s="20" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="N91" s="42" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.2">
@@ -5250,7 +5350,7 @@
         <v>107</v>
       </c>
       <c r="F92" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G92" s="20" t="s">
         <v>19</v>
@@ -5262,10 +5362,10 @@
       <c r="K92" s="33"/>
       <c r="L92" s="20"/>
       <c r="M92" s="20" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="N92" s="42" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.2">
@@ -5276,7 +5376,7 @@
         <v>105</v>
       </c>
       <c r="F93" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G93" s="20" t="s">
         <v>19</v>
@@ -5291,10 +5391,10 @@
       <c r="K93" s="33"/>
       <c r="L93" s="20"/>
       <c r="M93" s="20" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="N93" s="42" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.2">
@@ -5305,7 +5405,7 @@
         <v>103</v>
       </c>
       <c r="F94" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G94" s="20" t="s">
         <v>19</v>
@@ -5320,10 +5420,10 @@
       <c r="K94" s="33"/>
       <c r="L94" s="20"/>
       <c r="M94" s="20" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="N94" s="42" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.2">
@@ -5337,10 +5437,10 @@
         <v>100</v>
       </c>
       <c r="D95" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="F95" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G95" s="20" t="s">
         <v>19</v>
@@ -5355,10 +5455,10 @@
       <c r="K95" s="33"/>
       <c r="L95" s="20"/>
       <c r="M95" s="20" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="N95" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.2">
@@ -5372,10 +5472,10 @@
         <v>97</v>
       </c>
       <c r="D96" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="F96" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G96" s="20" t="s">
         <v>19</v>
@@ -5390,10 +5490,10 @@
       <c r="K96" s="33"/>
       <c r="L96" s="20"/>
       <c r="M96" s="20" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
       <c r="N96" s="42" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.2">
@@ -5407,10 +5507,10 @@
         <v>94</v>
       </c>
       <c r="D97" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="F97" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G97" s="20" t="s">
         <v>19</v>
@@ -5425,10 +5525,10 @@
       <c r="K97" s="33"/>
       <c r="L97" s="20"/>
       <c r="M97" s="20" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
       <c r="N97" s="42" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.2">
@@ -5442,7 +5542,7 @@
         <v>87</v>
       </c>
       <c r="F98" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G98" s="20" t="s">
         <v>19</v>
@@ -5457,10 +5557,10 @@
       <c r="K98" s="33"/>
       <c r="L98" s="20"/>
       <c r="M98" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N98" s="42" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.2">
@@ -5474,7 +5574,7 @@
         <v>87</v>
       </c>
       <c r="F99" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G99" s="20" t="s">
         <v>19</v>
@@ -5489,10 +5589,10 @@
       <c r="K99" s="33"/>
       <c r="L99" s="20"/>
       <c r="M99" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N99" s="42" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.2">
@@ -5506,7 +5606,7 @@
         <v>87</v>
       </c>
       <c r="F100" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G100" s="20" t="s">
         <v>19</v>
@@ -5521,10 +5621,10 @@
       <c r="K100" s="33"/>
       <c r="L100" s="20"/>
       <c r="M100" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N100" s="42" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.2">
@@ -5535,7 +5635,7 @@
         <v>85</v>
       </c>
       <c r="F101" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G101" s="20" t="s">
         <v>19</v>
@@ -5550,10 +5650,10 @@
       <c r="K101" s="33"/>
       <c r="L101" s="20"/>
       <c r="M101" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N101" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.2">
@@ -5564,7 +5664,7 @@
         <v>83</v>
       </c>
       <c r="F102" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G102" s="20" t="s">
         <v>19</v>
@@ -5579,10 +5679,10 @@
       <c r="K102" s="33"/>
       <c r="L102" s="20"/>
       <c r="M102" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N102" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.2">
@@ -5593,7 +5693,7 @@
         <v>81</v>
       </c>
       <c r="F103" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G103" s="20" t="s">
         <v>19</v>
@@ -5608,10 +5708,10 @@
       <c r="K103" s="33"/>
       <c r="L103" s="20"/>
       <c r="M103" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N103" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.2">
@@ -5622,7 +5722,7 @@
         <v>79</v>
       </c>
       <c r="F104" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G104" s="20" t="s">
         <v>19</v>
@@ -5637,10 +5737,10 @@
       <c r="K104" s="33"/>
       <c r="L104" s="20"/>
       <c r="M104" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N104" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.2">
@@ -5651,7 +5751,7 @@
         <v>77</v>
       </c>
       <c r="F105" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G105" s="20" t="s">
         <v>19</v>
@@ -5666,10 +5766,10 @@
       <c r="K105" s="33"/>
       <c r="L105" s="20"/>
       <c r="M105" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N105" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.2">
@@ -5680,7 +5780,7 @@
         <v>75</v>
       </c>
       <c r="F106" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G106" s="20" t="s">
         <v>19</v>
@@ -5695,10 +5795,10 @@
       <c r="K106" s="33"/>
       <c r="L106" s="20"/>
       <c r="M106" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N106" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.2">
@@ -5709,7 +5809,7 @@
         <v>73</v>
       </c>
       <c r="F107" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G107" s="20" t="s">
         <v>19</v>
@@ -5724,10 +5824,10 @@
       <c r="K107" s="33"/>
       <c r="L107" s="20"/>
       <c r="M107" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N107" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.2">
@@ -5738,7 +5838,7 @@
         <v>71</v>
       </c>
       <c r="F108" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G108" s="20" t="s">
         <v>19</v>
@@ -5753,10 +5853,10 @@
       <c r="K108" s="33"/>
       <c r="L108" s="20"/>
       <c r="M108" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="N108" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.2">
@@ -5770,7 +5870,7 @@
         <v>68</v>
       </c>
       <c r="F109" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G109" s="20" t="s">
         <v>19</v>
@@ -5785,10 +5885,10 @@
       <c r="K109" s="33"/>
       <c r="L109" s="20"/>
       <c r="M109" s="20" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="N109" s="42" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.2">
@@ -5802,7 +5902,7 @@
         <v>61</v>
       </c>
       <c r="F110" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G110" s="20" t="s">
         <v>19</v>
@@ -5817,10 +5917,10 @@
       <c r="K110" s="33"/>
       <c r="L110" s="20"/>
       <c r="M110" s="20" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="N110" s="42" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.2">
@@ -5834,7 +5934,7 @@
         <v>61</v>
       </c>
       <c r="F111" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G111" s="20" t="s">
         <v>19</v>
@@ -5849,10 +5949,10 @@
       <c r="K111" s="33"/>
       <c r="L111" s="20"/>
       <c r="M111" s="20" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="N111" s="42" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.2">
@@ -5868,7 +5968,7 @@
       <c r="D112" s="34"/>
       <c r="E112" s="20"/>
       <c r="F112" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G112" s="20" t="s">
         <v>19</v>
@@ -5883,10 +5983,10 @@
       <c r="K112" s="33"/>
       <c r="L112" s="20"/>
       <c r="M112" s="20" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="N112" s="42" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>